<commit_message>
Final Presentation Module 8
</commit_message>
<xml_diff>
--- a/Test.xlsx
+++ b/Test.xlsx
@@ -8,6 +8,11 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Statistics" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Bar Chart" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Line Chart" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Pie Chart" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Scatter Plot" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -136,7 +141,7 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:t>My Chart</a:t>
+              <a:t>Bar Chart Rank vs Coin name</a:t>
             </a:r>
           </a:p>
         </rich>
@@ -206,13 +211,354 @@
 </chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Line Chart Price vs Rank</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <lineChart>
+        <grouping val="standard"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'Sheet'!C1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <cat>
+            <numRef>
+              <f>'Sheet'!$B$2:$B$11</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Sheet'!$C$2:$C$11</f>
+            </numRef>
+          </val>
+        </ser>
+        <axId val="10"/>
+        <axId val="100"/>
+      </lineChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Pie Chart</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <pieChart>
+        <varyColors val="1"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'Pie Chart'!B2</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'Pie Chart'!$A$2:$A$5</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Pie Chart'!$B$3:$B$5</f>
+            </numRef>
+          </val>
+        </ser>
+        <firstSliceAng val="0"/>
+      </pieChart>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Scatter Plot of Rank vs Price</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <scatterChart>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <v>Price vs Rank Scatterplot</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Sheet'!$B$1:$B$11</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Sheet'!$C$1:$C$11</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <axId val="10"/>
+        <axId val="20"/>
+      </scatterChart>
+      <valAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Rank</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="20"/>
+      </valAx>
+      <valAx>
+        <axId val="20"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Price in Usd</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
-      <col>2</col>
+      <col>0</col>
       <colOff>0</colOff>
-      <row>4</row>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="1" name="Chart 1"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="1" name="Chart 1"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>3</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="1" name="Chart 1"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>0</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="5400000" cy="2700000"/>
@@ -522,7 +868,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B101"/>
+  <dimension ref="A1:C101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -541,6 +887,11 @@
           <t>Rank</t>
         </is>
       </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>priceUsd</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -551,6 +902,9 @@
       <c r="B2" t="n">
         <v>1</v>
       </c>
+      <c r="C2" t="n">
+        <v>96531.23026383475</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -561,6 +915,9 @@
       <c r="B3" t="n">
         <v>2</v>
       </c>
+      <c r="C3" t="n">
+        <v>3584.894738525208</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -571,6 +928,9 @@
       <c r="B4" t="n">
         <v>3</v>
       </c>
+      <c r="C4" t="n">
+        <v>1.000060416327784</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -581,6 +941,9 @@
       <c r="B5" t="n">
         <v>4</v>
       </c>
+      <c r="C5" t="n">
+        <v>241.9295590310666</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -591,6 +954,9 @@
       <c r="B6" t="n">
         <v>5</v>
       </c>
+      <c r="C6" t="n">
+        <v>658.4798856043273</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -601,6 +967,9 @@
       <c r="B7" t="n">
         <v>6</v>
       </c>
+      <c r="C7" t="n">
+        <v>1.554794012558481</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -611,6 +980,9 @@
       <c r="B8" t="n">
         <v>7</v>
       </c>
+      <c r="C8" t="n">
+        <v>0.406185874949573</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -621,26 +993,35 @@
       <c r="B9" t="n">
         <v>8</v>
       </c>
+      <c r="C9" t="n">
+        <v>0.9999756206499344</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Lido Staked ETH</t>
+          <t>Cardano</t>
         </is>
       </c>
       <c r="B10" t="n">
         <v>9</v>
       </c>
+      <c r="C10" t="n">
+        <v>1.049259051651274</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Cardano</t>
+          <t>Lido Staked ETH</t>
         </is>
       </c>
       <c r="B11" t="n">
         <v>10</v>
       </c>
+      <c r="C11" t="n">
+        <v>3565.834000514138</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -651,6 +1032,9 @@
       <c r="B12" t="n">
         <v>11</v>
       </c>
+      <c r="C12" t="n">
+        <v>43.36932025269478</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -661,6 +1045,9 @@
       <c r="B13" t="n">
         <v>12</v>
       </c>
+      <c r="C13" t="n">
+        <v>0.2019113057142266</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -671,6 +1058,9 @@
       <c r="B14" t="n">
         <v>13</v>
       </c>
+      <c r="C14" t="n">
+        <v>2.58394123006e-05</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -681,6 +1071,9 @@
       <c r="B15" t="n">
         <v>14</v>
       </c>
+      <c r="C15" t="n">
+        <v>0.4936473829147279</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -691,6 +1084,9 @@
       <c r="B16" t="n">
         <v>15</v>
       </c>
+      <c r="C16" t="n">
+        <v>96426.09578795652</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -701,6 +1097,9 @@
       <c r="B17" t="n">
         <v>16</v>
       </c>
+      <c r="C17" t="n">
+        <v>8.563198924333976</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -711,6 +1110,9 @@
       <c r="B18" t="n">
         <v>17</v>
       </c>
+      <c r="C18" t="n">
+        <v>17.82675872856533</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -721,6 +1123,9 @@
       <c r="B19" t="n">
         <v>18</v>
       </c>
+      <c r="C19" t="n">
+        <v>512.8863652253028</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -731,6 +1136,9 @@
       <c r="B20" t="n">
         <v>19</v>
       </c>
+      <c r="C20" t="n">
+        <v>6.826668708882036</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -741,6 +1149,9 @@
       <c r="B21" t="n">
         <v>20</v>
       </c>
+      <c r="C21" t="n">
+        <v>8.642617159181972</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -751,6 +1162,9 @@
       <c r="B22" t="n">
         <v>21</v>
       </c>
+      <c r="C22" t="n">
+        <v>12.61279224259548</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -761,36 +1175,48 @@
       <c r="B23" t="n">
         <v>22</v>
       </c>
+      <c r="C23" t="n">
+        <v>96.5638395748082</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Multi Collateral DAI</t>
+          <t>Internet Computer</t>
         </is>
       </c>
       <c r="B24" t="n">
         <v>23</v>
       </c>
+      <c r="C24" t="n">
+        <v>11.5169778166757</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Internet Computer</t>
+          <t>Sp8de</t>
         </is>
       </c>
       <c r="B25" t="n">
         <v>24</v>
       </c>
+      <c r="C25" t="n">
+        <v>0.695085253291207</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Sp8de</t>
+          <t>Multi Collateral DAI</t>
         </is>
       </c>
       <c r="B26" t="n">
         <v>25</v>
       </c>
+      <c r="C26" t="n">
+        <v>0.9992197826680486</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -801,6 +1227,9 @@
       <c r="B27" t="n">
         <v>26</v>
       </c>
+      <c r="C27" t="n">
+        <v>31.66284627173462</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -811,6 +1240,9 @@
       <c r="B28" t="n">
         <v>27</v>
       </c>
+      <c r="C28" t="n">
+        <v>0.1862713041499647</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -821,6 +1253,9 @@
       <c r="B29" t="n">
         <v>28</v>
       </c>
+      <c r="C29" t="n">
+        <v>1.600744439840803</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -831,6 +1266,9 @@
       <c r="B30" t="n">
         <v>29</v>
       </c>
+      <c r="C30" t="n">
+        <v>5.729477945719554</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -841,6 +1279,9 @@
       <c r="B31" t="n">
         <v>30</v>
       </c>
+      <c r="C31" t="n">
+        <v>2.279996291522955</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -851,6 +1292,9 @@
       <c r="B32" t="n">
         <v>31</v>
       </c>
+      <c r="C32" t="n">
+        <v>0.0420265564219433</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -861,86 +1305,113 @@
       <c r="B33" t="n">
         <v>32</v>
       </c>
+      <c r="C33" t="n">
+        <v>199.1954044169622</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Fantom</t>
+          <t>Algorand</t>
         </is>
       </c>
       <c r="B34" t="n">
         <v>33</v>
       </c>
+      <c r="C34" t="n">
+        <v>0.3535321456730872</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Monero</t>
+          <t>Fantom</t>
         </is>
       </c>
       <c r="B35" t="n">
         <v>34</v>
       </c>
+      <c r="C35" t="n">
+        <v>1.029769916787292</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>The Graph</t>
+          <t>Monero</t>
         </is>
       </c>
       <c r="B36" t="n">
         <v>35</v>
       </c>
+      <c r="C36" t="n">
+        <v>156.1281119312631</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Algorand</t>
+          <t>The Graph</t>
         </is>
       </c>
       <c r="B37" t="n">
         <v>36</v>
       </c>
+      <c r="C37" t="n">
+        <v>0.2662996885934634</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Injective</t>
+          <t>Hedera Hashgraph</t>
         </is>
       </c>
       <c r="B38" t="n">
         <v>37</v>
       </c>
+      <c r="C38" t="n">
+        <v>0.1499435396494146</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Hedera Hashgraph</t>
+          <t>Injective</t>
         </is>
       </c>
       <c r="B39" t="n">
         <v>38</v>
       </c>
+      <c r="C39" t="n">
+        <v>29.81491593278191</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Cosmos</t>
+          <t>THETA</t>
         </is>
       </c>
       <c r="B40" t="n">
         <v>39</v>
       </c>
+      <c r="C40" t="n">
+        <v>2.15584010125914</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>THETA</t>
+          <t>Cosmos</t>
         </is>
       </c>
       <c r="B41" t="n">
         <v>40</v>
       </c>
+      <c r="C41" t="n">
+        <v>8.240489266822495</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -951,6 +1422,9 @@
       <c r="B42" t="n">
         <v>41</v>
       </c>
+      <c r="C42" t="n">
+        <v>5.592307966847702</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -961,76 +1435,100 @@
       <c r="B43" t="n">
         <v>42</v>
       </c>
+      <c r="C43" t="n">
+        <v>3.629145464161419</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Maker</t>
+          <t>Raydium</t>
         </is>
       </c>
       <c r="B44" t="n">
         <v>43</v>
       </c>
+      <c r="C44" t="n">
+        <v>5.850032567630714</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Raydium</t>
+          <t>Maker</t>
         </is>
       </c>
       <c r="B45" t="n">
         <v>44</v>
       </c>
+      <c r="C45" t="n">
+        <v>1836.126877313236</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Lido DAO</t>
+          <t>The Sandbox</t>
         </is>
       </c>
       <c r="B46" t="n">
         <v>45</v>
       </c>
+      <c r="C46" t="n">
+        <v>0.6586684263364017</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>The Sandbox</t>
+          <t>Lido DAO</t>
         </is>
       </c>
       <c r="B47" t="n">
         <v>46</v>
       </c>
+      <c r="C47" t="n">
+        <v>1.724948381770404</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>KuCoin Token</t>
+          <t>Arweave</t>
         </is>
       </c>
       <c r="B48" t="n">
         <v>47</v>
       </c>
+      <c r="C48" t="n">
+        <v>21.54180830486543</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Bitcoin SV</t>
+          <t>KuCoin Token</t>
         </is>
       </c>
       <c r="B49" t="n">
         <v>48</v>
       </c>
+      <c r="C49" t="n">
+        <v>11.63462231645978</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Arweave</t>
+          <t>Gala</t>
         </is>
       </c>
       <c r="B50" t="n">
         <v>49</v>
       </c>
+      <c r="C50" t="n">
+        <v>0.0388374693048543</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -1041,16 +1539,22 @@
       <c r="B51" t="n">
         <v>50</v>
       </c>
+      <c r="C51" t="n">
+        <v>0.8916896494645306</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Gala</t>
+          <t>Bitcoin SV</t>
         </is>
       </c>
       <c r="B52" t="n">
         <v>51</v>
       </c>
+      <c r="C52" t="n">
+        <v>69.6755555434175</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -1061,6 +1565,9 @@
       <c r="B53" t="n">
         <v>52</v>
       </c>
+      <c r="C53" t="n">
+        <v>1.263085481518663</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -1071,6 +1578,9 @@
       <c r="B54" t="n">
         <v>53</v>
       </c>
+      <c r="C54" t="n">
+        <v>0.5604354497574325</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -1081,26 +1591,35 @@
       <c r="B55" t="n">
         <v>54</v>
       </c>
+      <c r="C55" t="n">
+        <v>0.8089676694783563</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Axie Infinity</t>
+          <t>Decentraland</t>
         </is>
       </c>
       <c r="B56" t="n">
         <v>55</v>
       </c>
+      <c r="C56" t="n">
+        <v>0.6305213606373605</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Decentraland</t>
+          <t>Axie Infinity</t>
         </is>
       </c>
       <c r="B57" t="n">
         <v>56</v>
       </c>
+      <c r="C57" t="n">
+        <v>7.851844142889142</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -1111,6 +1630,9 @@
       <c r="B58" t="n">
         <v>57</v>
       </c>
+      <c r="C58" t="n">
+        <v>95.11260152029415</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -1121,36 +1643,48 @@
       <c r="B59" t="n">
         <v>58</v>
       </c>
+      <c r="C59" t="n">
+        <v>6.511178771048733</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Neo</t>
+          <t>Akash Network</t>
         </is>
       </c>
       <c r="B60" t="n">
         <v>59</v>
       </c>
+      <c r="C60" t="n">
+        <v>4.268181331727236</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>GateToken</t>
+          <t>Neo</t>
         </is>
       </c>
       <c r="B61" t="n">
         <v>60</v>
       </c>
+      <c r="C61" t="n">
+        <v>14.66543796452646</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Akash Network</t>
+          <t>GateToken</t>
         </is>
       </c>
       <c r="B62" t="n">
         <v>61</v>
       </c>
+      <c r="C62" t="n">
+        <v>11.49879094627228</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -1161,16 +1695,22 @@
       <c r="B63" t="n">
         <v>62</v>
       </c>
+      <c r="C63" t="n">
+        <v>4.85003370641e-05</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Mina</t>
+          <t>MultiversX</t>
         </is>
       </c>
       <c r="B64" t="n">
         <v>63</v>
       </c>
+      <c r="C64" t="n">
+        <v>39.64794050440727</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -1181,76 +1721,100 @@
       <c r="B65" t="n">
         <v>64</v>
       </c>
+      <c r="C65" t="n">
+        <v>56.1439301885075</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Nexo</t>
+          <t>Mina</t>
         </is>
       </c>
       <c r="B66" t="n">
         <v>65</v>
       </c>
+      <c r="C66" t="n">
+        <v>0.7690409134251464</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>MultiversX</t>
+          <t>Pendle</t>
         </is>
       </c>
       <c r="B67" t="n">
         <v>66</v>
       </c>
+      <c r="C67" t="n">
+        <v>5.509063379044178</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Pendle</t>
+          <t>AIOZ Network</t>
         </is>
       </c>
       <c r="B68" t="n">
         <v>67</v>
       </c>
+      <c r="C68" t="n">
+        <v>0.7942009352051562</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>PancakeSwap</t>
+          <t>Nexo</t>
         </is>
       </c>
       <c r="B69" t="n">
         <v>68</v>
       </c>
+      <c r="C69" t="n">
+        <v>1.399365277653627</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>AIOZ Network</t>
+          <t>Conflux</t>
         </is>
       </c>
       <c r="B70" t="n">
         <v>69</v>
       </c>
+      <c r="C70" t="n">
+        <v>0.1872823773424943</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Conflux</t>
+          <t>Chiliz</t>
         </is>
       </c>
       <c r="B71" t="n">
         <v>70</v>
       </c>
+      <c r="C71" t="n">
+        <v>0.09374447265871649</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Chiliz</t>
+          <t>PancakeSwap</t>
         </is>
       </c>
       <c r="B72" t="n">
         <v>71</v>
       </c>
+      <c r="C72" t="n">
+        <v>3.014141670463326</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -1261,6 +1825,9 @@
       <c r="B73" t="n">
         <v>72</v>
       </c>
+      <c r="C73" t="n">
+        <v>0.234176891323387</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -1271,46 +1838,61 @@
       <c r="B74" t="n">
         <v>73</v>
       </c>
+      <c r="C74" t="n">
+        <v>2.28626170791341</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Gnosis</t>
+          <t>Nervos Network</t>
         </is>
       </c>
       <c r="B75" t="n">
         <v>74</v>
       </c>
+      <c r="C75" t="n">
+        <v>0.0153054901867988</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Nervos Network</t>
+          <t>Gnosis</t>
         </is>
       </c>
       <c r="B76" t="n">
         <v>75</v>
       </c>
+      <c r="C76" t="n">
+        <v>268.074090883717</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>XinFin Network</t>
+          <t>Oasis</t>
         </is>
       </c>
       <c r="B77" t="n">
         <v>76</v>
       </c>
+      <c r="C77" t="n">
+        <v>0.09633516844841621</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Oasis</t>
+          <t>XinFin Network</t>
         </is>
       </c>
       <c r="B78" t="n">
         <v>77</v>
       </c>
+      <c r="C78" t="n">
+        <v>0.0543587736267139</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -1321,6 +1903,9 @@
       <c r="B79" t="n">
         <v>78</v>
       </c>
+      <c r="C79" t="n">
+        <v>1.327141463264847</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -1331,6 +1916,9 @@
       <c r="B80" t="n">
         <v>79</v>
       </c>
+      <c r="C80" t="n">
+        <v>70.97241346446538</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -1341,6 +1929,9 @@
       <c r="B81" t="n">
         <v>80</v>
       </c>
+      <c r="C81" t="n">
+        <v>0.5050872747285243</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -1351,6 +1942,9 @@
       <c r="B82" t="n">
         <v>81</v>
       </c>
+      <c r="C82" t="n">
+        <v>0.5421528425481286</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -1361,76 +1955,100 @@
       <c r="B83" t="n">
         <v>82</v>
       </c>
+      <c r="C83" t="n">
+        <v>37.13569464495722</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Synthetix</t>
+          <t>Amp</t>
         </is>
       </c>
       <c r="B84" t="n">
         <v>83</v>
       </c>
+      <c r="C84" t="n">
+        <v>0.0071480411212037</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>1inch Network</t>
+          <t>Synthetix</t>
         </is>
       </c>
       <c r="B85" t="n">
         <v>84</v>
       </c>
+      <c r="C85" t="n">
+        <v>2.358612253354329</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Theta Fuel</t>
+          <t>1inch Network</t>
         </is>
       </c>
       <c r="B86" t="n">
         <v>85</v>
       </c>
+      <c r="C86" t="n">
+        <v>0.4137882041021117</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>NXM</t>
+          <t>Livepeer</t>
         </is>
       </c>
       <c r="B87" t="n">
         <v>86</v>
       </c>
+      <c r="C87" t="n">
+        <v>14.84910940308136</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Livepeer</t>
+          <t>Theta Fuel</t>
         </is>
       </c>
       <c r="B88" t="n">
         <v>87</v>
       </c>
+      <c r="C88" t="n">
+        <v>0.07857579313037689</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>TrueUSD</t>
+          <t>Telcoin</t>
         </is>
       </c>
       <c r="B89" t="n">
         <v>88</v>
       </c>
+      <c r="C89" t="n">
+        <v>0.0057034448480341</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Holo</t>
+          <t>Enjin Coin</t>
         </is>
       </c>
       <c r="B90" t="n">
         <v>89</v>
       </c>
+      <c r="C90" t="n">
+        <v>0.2881698743164208</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -1441,46 +2059,61 @@
       <c r="B91" t="n">
         <v>90</v>
       </c>
+      <c r="C91" t="n">
+        <v>0.2760413709747691</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>Enjin Coin</t>
+          <t>Holo</t>
         </is>
       </c>
       <c r="B92" t="n">
         <v>91</v>
       </c>
+      <c r="C92" t="n">
+        <v>0.0028964692028345</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>Amp</t>
+          <t>NXM</t>
         </is>
       </c>
       <c r="B93" t="n">
         <v>92</v>
       </c>
+      <c r="C93" t="n">
+        <v>75.71350556613712</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>DeXe</t>
+          <t>TrueUSD</t>
         </is>
       </c>
       <c r="B94" t="n">
         <v>93</v>
       </c>
+      <c r="C94" t="n">
+        <v>1.001591030172031</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>Zilliqa</t>
+          <t>DeXe</t>
         </is>
       </c>
       <c r="B95" t="n">
         <v>94</v>
       </c>
+      <c r="C95" t="n">
+        <v>8.643956462393321</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -1491,59 +2124,242 @@
       <c r="B96" t="n">
         <v>95</v>
       </c>
+      <c r="C96" t="n">
+        <v>0.009017443943484801</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>Telcoin</t>
+          <t>Zilliqa</t>
         </is>
       </c>
       <c r="B97" t="n">
         <v>96</v>
       </c>
+      <c r="C97" t="n">
+        <v>0.02491895061678</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>0x Protocol</t>
+          <t>Golem</t>
         </is>
       </c>
       <c r="B98" t="n">
         <v>97</v>
       </c>
+      <c r="C98" t="n">
+        <v>0.4778649501424878</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>Golem</t>
+          <t>Trust Wallet Token</t>
         </is>
       </c>
       <c r="B99" t="n">
         <v>98</v>
       </c>
+      <c r="C99" t="n">
+        <v>1.145727847981554</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>Celo</t>
+          <t>0x Protocol</t>
         </is>
       </c>
       <c r="B100" t="n">
         <v>99</v>
       </c>
+      <c r="C100" t="n">
+        <v>0.5508921118380792</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>Trust Wallet Token</t>
+          <t>IoTeX</t>
         </is>
       </c>
       <c r="B101" t="n">
         <v>100</v>
+      </c>
+      <c r="C101" t="n">
+        <v>0.0484214435297264</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Mean</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Median</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>std</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>2048.7</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="C2" t="n">
+        <v>13568.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Categories</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>PERCENTAGE</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Category 1</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Category 2</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Category 3</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Last and Final Revision: 2024.12.03
</commit_message>
<xml_diff>
--- a/Test.xlsx
+++ b/Test.xlsx
@@ -903,7 +903,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>96531.23026383475</v>
+        <v>95706.12940484812</v>
       </c>
     </row>
     <row r="3">
@@ -916,7 +916,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>3584.894738525208</v>
+        <v>3647.614127816061</v>
       </c>
     </row>
     <row r="4">
@@ -929,46 +929,46 @@
         <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>1.000060416327784</v>
+        <v>1.00029194544417</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Solana</t>
+          <t>BNB</t>
         </is>
       </c>
       <c r="B5" t="n">
         <v>4</v>
       </c>
       <c r="C5" t="n">
-        <v>241.9295590310666</v>
+        <v>751.5138343936801</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>BNB</t>
+          <t>XRP</t>
         </is>
       </c>
       <c r="B6" t="n">
         <v>5</v>
       </c>
       <c r="C6" t="n">
-        <v>658.4798856043273</v>
+        <v>2.517656103469206</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>XRP</t>
+          <t>Solana</t>
         </is>
       </c>
       <c r="B7" t="n">
         <v>6</v>
       </c>
       <c r="C7" t="n">
-        <v>1.554794012558481</v>
+        <v>236.1708739410761</v>
       </c>
     </row>
     <row r="8">
@@ -981,33 +981,33 @@
         <v>7</v>
       </c>
       <c r="C8" t="n">
-        <v>0.406185874949573</v>
+        <v>0.4124796933033013</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>USDC</t>
+          <t>Cardano</t>
         </is>
       </c>
       <c r="B9" t="n">
         <v>8</v>
       </c>
       <c r="C9" t="n">
-        <v>0.9999756206499344</v>
+        <v>1.196424070616533</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Cardano</t>
+          <t>USDC</t>
         </is>
       </c>
       <c r="B10" t="n">
         <v>9</v>
       </c>
       <c r="C10" t="n">
-        <v>1.049259051651274</v>
+        <v>0.999887564710715</v>
       </c>
     </row>
     <row r="11">
@@ -1020,33 +1020,33 @@
         <v>10</v>
       </c>
       <c r="C11" t="n">
-        <v>3565.834000514138</v>
+        <v>3620.467876837743</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Avalanche</t>
+          <t>TRON</t>
         </is>
       </c>
       <c r="B12" t="n">
         <v>11</v>
       </c>
       <c r="C12" t="n">
-        <v>43.36932025269478</v>
+        <v>0.3745805180736099</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>TRON</t>
+          <t>Avalanche</t>
         </is>
       </c>
       <c r="B13" t="n">
         <v>12</v>
       </c>
       <c r="C13" t="n">
-        <v>0.2019113057142266</v>
+        <v>51.45218344200527</v>
       </c>
     </row>
     <row r="14">
@@ -1059,7 +1059,7 @@
         <v>13</v>
       </c>
       <c r="C14" t="n">
-        <v>2.58394123006e-05</v>
+        <v>2.99999301083e-05</v>
       </c>
     </row>
     <row r="15">
@@ -1072,20 +1072,20 @@
         <v>14</v>
       </c>
       <c r="C15" t="n">
-        <v>0.4936473829147279</v>
+        <v>0.5061716247575836</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Wrapped Bitcoin</t>
+          <t>Chainlink</t>
         </is>
       </c>
       <c r="B16" t="n">
         <v>15</v>
       </c>
       <c r="C16" t="n">
-        <v>96426.09578795652</v>
+        <v>23.74415752206779</v>
       </c>
     </row>
     <row r="17">
@@ -1098,20 +1098,20 @@
         <v>16</v>
       </c>
       <c r="C17" t="n">
-        <v>8.563198924333976</v>
+        <v>9.753780387062024</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Chainlink</t>
+          <t>Wrapped Bitcoin</t>
         </is>
       </c>
       <c r="B18" t="n">
         <v>17</v>
       </c>
       <c r="C18" t="n">
-        <v>17.82675872856533</v>
+        <v>95444.4697948156</v>
       </c>
     </row>
     <row r="19">
@@ -1124,59 +1124,59 @@
         <v>18</v>
       </c>
       <c r="C19" t="n">
-        <v>512.8863652253028</v>
+        <v>564.7635566181027</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>NEAR Protocol</t>
+          <t>Litecoin</t>
         </is>
       </c>
       <c r="B20" t="n">
         <v>19</v>
       </c>
       <c r="C20" t="n">
-        <v>6.826668708882036</v>
+        <v>128.4899641654699</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>UNUS SED LEO</t>
+          <t>Uniswap</t>
         </is>
       </c>
       <c r="B21" t="n">
         <v>20</v>
       </c>
       <c r="C21" t="n">
-        <v>8.642617159181972</v>
+        <v>14.72264708288165</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Uniswap</t>
+          <t>NEAR Protocol</t>
         </is>
       </c>
       <c r="B22" t="n">
         <v>21</v>
       </c>
       <c r="C22" t="n">
-        <v>12.61279224259548</v>
+        <v>7.230190371054206</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Litecoin</t>
+          <t>UNUS SED LEO</t>
         </is>
       </c>
       <c r="B23" t="n">
         <v>22</v>
       </c>
       <c r="C23" t="n">
-        <v>96.5638395748082</v>
+        <v>9.378120456024803</v>
       </c>
     </row>
     <row r="24">
@@ -1189,20 +1189,20 @@
         <v>23</v>
       </c>
       <c r="C24" t="n">
-        <v>11.5169778166757</v>
+        <v>14.30680728225584</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Sp8de</t>
+          <t>VeChain</t>
         </is>
       </c>
       <c r="B25" t="n">
         <v>24</v>
       </c>
       <c r="C25" t="n">
-        <v>0.695085253291207</v>
+        <v>0.0713035356852022</v>
       </c>
     </row>
     <row r="26">
@@ -1215,7 +1215,7 @@
         <v>25</v>
       </c>
       <c r="C26" t="n">
-        <v>0.9992197826680486</v>
+        <v>0.9997725402354023</v>
       </c>
     </row>
     <row r="27">
@@ -1228,7 +1228,7 @@
         <v>26</v>
       </c>
       <c r="C27" t="n">
-        <v>31.66284627173462</v>
+        <v>35.5635463814456</v>
       </c>
     </row>
     <row r="28">
@@ -1241,150 +1241,150 @@
         <v>27</v>
       </c>
       <c r="C28" t="n">
-        <v>0.1862713041499647</v>
+        <v>0.1989262583227424</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Artificial Superintelligence Alliance</t>
+          <t>Sp8de</t>
         </is>
       </c>
       <c r="B29" t="n">
         <v>28</v>
       </c>
       <c r="C29" t="n">
-        <v>1.600744439840803</v>
+        <v>0.6305730521682377</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Filecoin</t>
+          <t>Hedera Hashgraph</t>
         </is>
       </c>
       <c r="B30" t="n">
         <v>29</v>
       </c>
       <c r="C30" t="n">
-        <v>5.729477945719554</v>
+        <v>0.3230489095306408</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Stacks</t>
+          <t>Artificial Superintelligence Alliance</t>
         </is>
       </c>
       <c r="B31" t="n">
         <v>30</v>
       </c>
       <c r="C31" t="n">
-        <v>2.279996291522955</v>
+        <v>1.899088648975919</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>VeChain</t>
+          <t>Filecoin</t>
         </is>
       </c>
       <c r="B32" t="n">
         <v>31</v>
       </c>
       <c r="C32" t="n">
-        <v>0.0420265564219433</v>
+        <v>7.50177219157705</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Aave</t>
+          <t>Algorand</t>
         </is>
       </c>
       <c r="B33" t="n">
         <v>32</v>
       </c>
       <c r="C33" t="n">
-        <v>199.1954044169622</v>
+        <v>0.5225528938049699</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Algorand</t>
+          <t>Stacks</t>
         </is>
       </c>
       <c r="B34" t="n">
         <v>33</v>
       </c>
       <c r="C34" t="n">
-        <v>0.3535321456730872</v>
+        <v>2.568231338139122</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Fantom</t>
+          <t>Monero</t>
         </is>
       </c>
       <c r="B35" t="n">
         <v>34</v>
       </c>
       <c r="C35" t="n">
-        <v>1.029769916787292</v>
+        <v>199.1759878162702</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Monero</t>
+          <t>OKB</t>
         </is>
       </c>
       <c r="B36" t="n">
         <v>35</v>
       </c>
       <c r="C36" t="n">
-        <v>156.1281119312631</v>
+        <v>60.76082907329035</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>The Graph</t>
+          <t>Aave</t>
         </is>
       </c>
       <c r="B37" t="n">
         <v>36</v>
       </c>
       <c r="C37" t="n">
-        <v>0.2662996885934634</v>
+        <v>238.8627715284042</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Hedera Hashgraph</t>
+          <t>Fantom</t>
         </is>
       </c>
       <c r="B38" t="n">
         <v>37</v>
       </c>
       <c r="C38" t="n">
-        <v>0.1499435396494146</v>
+        <v>1.234611448289417</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Injective</t>
+          <t>The Graph</t>
         </is>
       </c>
       <c r="B39" t="n">
         <v>38</v>
       </c>
       <c r="C39" t="n">
-        <v>29.81491593278191</v>
+        <v>0.3119893596470023</v>
       </c>
     </row>
     <row r="40">
@@ -1397,59 +1397,59 @@
         <v>39</v>
       </c>
       <c r="C40" t="n">
-        <v>2.15584010125914</v>
+        <v>2.92134492588411</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Cosmos</t>
+          <t>Injective</t>
         </is>
       </c>
       <c r="B41" t="n">
         <v>40</v>
       </c>
       <c r="C41" t="n">
-        <v>8.240489266822495</v>
+        <v>32.79218321236868</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>THORChain</t>
+          <t>Cosmos</t>
         </is>
       </c>
       <c r="B42" t="n">
         <v>41</v>
       </c>
       <c r="C42" t="n">
-        <v>5.592307966847702</v>
+        <v>9.50312939339447</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>MANTRA DAO</t>
+          <t>THORChain</t>
         </is>
       </c>
       <c r="B43" t="n">
         <v>42</v>
       </c>
       <c r="C43" t="n">
-        <v>3.629145464161419</v>
+        <v>6.813167763105839</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Raydium</t>
+          <t>EOS</t>
         </is>
       </c>
       <c r="B44" t="n">
         <v>43</v>
       </c>
       <c r="C44" t="n">
-        <v>5.850032567630714</v>
+        <v>1.439464472980603</v>
       </c>
     </row>
     <row r="45">
@@ -1462,72 +1462,72 @@
         <v>44</v>
       </c>
       <c r="C45" t="n">
-        <v>1836.126877313236</v>
+        <v>2320.27761085187</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>The Sandbox</t>
+          <t>IOTA</t>
         </is>
       </c>
       <c r="B46" t="n">
         <v>45</v>
       </c>
       <c r="C46" t="n">
-        <v>0.6586684263364017</v>
+        <v>0.5799393202739836</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Lido DAO</t>
+          <t>MANTRA DAO</t>
         </is>
       </c>
       <c r="B47" t="n">
         <v>46</v>
       </c>
       <c r="C47" t="n">
-        <v>1.724948381770404</v>
+        <v>3.865202862651067</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Arweave</t>
+          <t>The Sandbox</t>
         </is>
       </c>
       <c r="B48" t="n">
         <v>47</v>
       </c>
       <c r="C48" t="n">
-        <v>21.54180830486543</v>
+        <v>0.7688972455961697</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>KuCoin Token</t>
+          <t>Gala</t>
         </is>
       </c>
       <c r="B49" t="n">
         <v>48</v>
       </c>
       <c r="C49" t="n">
-        <v>11.63462231645978</v>
+        <v>0.0511291384015356</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Gala</t>
+          <t>Lido DAO</t>
         </is>
       </c>
       <c r="B50" t="n">
         <v>49</v>
       </c>
       <c r="C50" t="n">
-        <v>0.0388374693048543</v>
+        <v>2.040327398783852</v>
       </c>
     </row>
     <row r="51">
@@ -1540,332 +1540,332 @@
         <v>50</v>
       </c>
       <c r="C51" t="n">
-        <v>0.8916896494645306</v>
+        <v>1.153409346194165</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Bitcoin SV</t>
+          <t>Arweave</t>
         </is>
       </c>
       <c r="B52" t="n">
         <v>51</v>
       </c>
       <c r="C52" t="n">
-        <v>69.6755555434175</v>
+        <v>27.18831590262465</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Tezos</t>
+          <t>Quant</t>
         </is>
       </c>
       <c r="B53" t="n">
         <v>52</v>
       </c>
       <c r="C53" t="n">
-        <v>1.263085481518663</v>
+        <v>142.5754269695325</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Polygon</t>
+          <t>Tezos</t>
         </is>
       </c>
       <c r="B54" t="n">
         <v>53</v>
       </c>
       <c r="C54" t="n">
-        <v>0.5604354497574325</v>
+        <v>1.689243969923392</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>EOS</t>
+          <t>Neo</t>
         </is>
       </c>
       <c r="B55" t="n">
         <v>54</v>
       </c>
       <c r="C55" t="n">
-        <v>0.8089676694783563</v>
+        <v>23.09408529776423</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Decentraland</t>
+          <t>Polygon</t>
         </is>
       </c>
       <c r="B56" t="n">
         <v>55</v>
       </c>
       <c r="C56" t="n">
-        <v>0.6305213606373605</v>
+        <v>0.7042263434138653</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Axie Infinity</t>
+          <t>KuCoin Token</t>
         </is>
       </c>
       <c r="B57" t="n">
         <v>56</v>
       </c>
       <c r="C57" t="n">
-        <v>7.851844142889142</v>
+        <v>12.86631767220504</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Quant</t>
+          <t>Helium</t>
         </is>
       </c>
       <c r="B58" t="n">
         <v>57</v>
       </c>
       <c r="C58" t="n">
-        <v>95.11260152029415</v>
+        <v>8.880404548421943</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Helium</t>
+          <t>Bitcoin SV</t>
         </is>
       </c>
       <c r="B59" t="n">
         <v>58</v>
       </c>
       <c r="C59" t="n">
-        <v>6.511178771048733</v>
+        <v>76.08217931632423</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Akash Network</t>
+          <t>Raydium</t>
         </is>
       </c>
       <c r="B60" t="n">
         <v>59</v>
       </c>
       <c r="C60" t="n">
-        <v>4.268181331727236</v>
+        <v>5.070599069983644</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Neo</t>
+          <t>Axie Infinity</t>
         </is>
       </c>
       <c r="B61" t="n">
         <v>60</v>
       </c>
       <c r="C61" t="n">
-        <v>14.66543796452646</v>
+        <v>9.201375304239761</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>GateToken</t>
+          <t>Decentraland</t>
         </is>
       </c>
       <c r="B62" t="n">
         <v>61</v>
       </c>
       <c r="C62" t="n">
-        <v>11.49879094627228</v>
+        <v>0.6905579344804675</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>eCash</t>
+          <t>MultiversX</t>
         </is>
       </c>
       <c r="B63" t="n">
         <v>62</v>
       </c>
       <c r="C63" t="n">
-        <v>4.85003370641e-05</v>
+        <v>52.56985537178777</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>MultiversX</t>
+          <t>AIOZ Network</t>
         </is>
       </c>
       <c r="B64" t="n">
         <v>63</v>
       </c>
       <c r="C64" t="n">
-        <v>39.64794050440727</v>
+        <v>1.111713337277815</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Zcash</t>
+          <t>Conflux</t>
         </is>
       </c>
       <c r="B65" t="n">
         <v>64</v>
       </c>
       <c r="C65" t="n">
-        <v>56.1439301885075</v>
+        <v>0.2556315291398551</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Mina</t>
+          <t>Zcash</t>
         </is>
       </c>
       <c r="B66" t="n">
         <v>65</v>
       </c>
       <c r="C66" t="n">
-        <v>0.7690409134251464</v>
+        <v>72.41205538679591</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Pendle</t>
+          <t>GateToken</t>
         </is>
       </c>
       <c r="B67" t="n">
         <v>66</v>
       </c>
       <c r="C67" t="n">
-        <v>5.509063379044178</v>
+        <v>12.70939935618371</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>AIOZ Network</t>
+          <t>Reserve Rights</t>
         </is>
       </c>
       <c r="B68" t="n">
         <v>67</v>
       </c>
       <c r="C68" t="n">
-        <v>0.7942009352051562</v>
+        <v>0.0209272965523953</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Nexo</t>
+          <t>Chiliz</t>
         </is>
       </c>
       <c r="B69" t="n">
         <v>68</v>
       </c>
       <c r="C69" t="n">
-        <v>1.399365277653627</v>
+        <v>0.1193086562992418</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Conflux</t>
+          <t>Mina</t>
         </is>
       </c>
       <c r="B70" t="n">
         <v>69</v>
       </c>
       <c r="C70" t="n">
-        <v>0.1872823773424943</v>
+        <v>0.9173660555248648</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Chiliz</t>
+          <t>Curve DAO Token</t>
         </is>
       </c>
       <c r="B71" t="n">
         <v>70</v>
       </c>
       <c r="C71" t="n">
-        <v>0.09374447265871649</v>
+        <v>0.8747312753173011</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>PancakeSwap</t>
+          <t>eCash</t>
         </is>
       </c>
       <c r="B72" t="n">
         <v>71</v>
       </c>
       <c r="C72" t="n">
-        <v>3.014141670463326</v>
+        <v>5.39320011504e-05</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>IOTA</t>
+          <t>Akash Network</t>
         </is>
       </c>
       <c r="B73" t="n">
         <v>72</v>
       </c>
       <c r="C73" t="n">
-        <v>0.234176891323387</v>
+        <v>4.256929732800584</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>FTX Token</t>
+          <t>Pendle</t>
         </is>
       </c>
       <c r="B74" t="n">
         <v>73</v>
       </c>
       <c r="C74" t="n">
-        <v>2.28626170791341</v>
+        <v>6.36759257895398</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Nervos Network</t>
+          <t>PancakeSwap</t>
         </is>
       </c>
       <c r="B75" t="n">
         <v>74</v>
       </c>
       <c r="C75" t="n">
-        <v>0.0153054901867988</v>
+        <v>3.52424150719294</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Gnosis</t>
+          <t>XinFin Network</t>
         </is>
       </c>
       <c r="B76" t="n">
         <v>75</v>
       </c>
       <c r="C76" t="n">
-        <v>268.074090883717</v>
+        <v>0.07811543886775341</v>
       </c>
     </row>
     <row r="77">
@@ -1878,319 +1878,319 @@
         <v>76</v>
       </c>
       <c r="C77" t="n">
-        <v>0.09633516844841621</v>
+        <v>0.1358193749089508</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>XinFin Network</t>
+          <t>Nexo</t>
         </is>
       </c>
       <c r="B78" t="n">
         <v>77</v>
       </c>
       <c r="C78" t="n">
-        <v>0.0543587736267139</v>
+        <v>1.479580060794976</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>SuperVerse</t>
+          <t>Amp</t>
         </is>
       </c>
       <c r="B79" t="n">
         <v>78</v>
       </c>
       <c r="C79" t="n">
-        <v>1.327141463264847</v>
+        <v>0.0117482380443289</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Compound</t>
+          <t>FTX Token</t>
         </is>
       </c>
       <c r="B80" t="n">
         <v>79</v>
       </c>
       <c r="C80" t="n">
-        <v>70.97241346446538</v>
+        <v>2.724066151435012</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Curve DAO Token</t>
+          <t>SuperVerse</t>
         </is>
       </c>
       <c r="B81" t="n">
         <v>80</v>
       </c>
       <c r="C81" t="n">
-        <v>0.5050872747285243</v>
+        <v>1.703215909235181</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Kava</t>
+          <t>Nervos Network</t>
         </is>
       </c>
       <c r="B82" t="n">
         <v>81</v>
       </c>
       <c r="C82" t="n">
-        <v>0.5421528425481286</v>
+        <v>0.0179734077664143</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Kusama</t>
+          <t>Compound</t>
         </is>
       </c>
       <c r="B83" t="n">
         <v>82</v>
       </c>
       <c r="C83" t="n">
-        <v>37.13569464495722</v>
+        <v>87.33242034194339</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Amp</t>
+          <t>Kava</t>
         </is>
       </c>
       <c r="B84" t="n">
         <v>83</v>
       </c>
       <c r="C84" t="n">
-        <v>0.0071480411212037</v>
+        <v>0.6889598030884678</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Synthetix</t>
+          <t>Gnosis</t>
         </is>
       </c>
       <c r="B85" t="n">
         <v>84</v>
       </c>
       <c r="C85" t="n">
-        <v>2.358612253354329</v>
+        <v>277.4327337683155</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>1inch Network</t>
+          <t>Kusama</t>
         </is>
       </c>
       <c r="B86" t="n">
         <v>85</v>
       </c>
       <c r="C86" t="n">
-        <v>0.4137882041021117</v>
+        <v>43.81442483102403</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Livepeer</t>
+          <t>Dash</t>
         </is>
       </c>
       <c r="B87" t="n">
         <v>86</v>
       </c>
       <c r="C87" t="n">
-        <v>14.84910940308136</v>
+        <v>56.78322048768199</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Theta Fuel</t>
+          <t>1inch Network</t>
         </is>
       </c>
       <c r="B88" t="n">
         <v>87</v>
       </c>
       <c r="C88" t="n">
-        <v>0.07857579313037689</v>
+        <v>0.5152824568864862</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>Telcoin</t>
+          <t>Synthetix</t>
         </is>
       </c>
       <c r="B89" t="n">
         <v>88</v>
       </c>
       <c r="C89" t="n">
-        <v>0.0057034448480341</v>
+        <v>2.86570576768944</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Enjin Coin</t>
+          <t>Zilliqa</t>
         </is>
       </c>
       <c r="B90" t="n">
         <v>89</v>
       </c>
       <c r="C90" t="n">
-        <v>0.2881698743164208</v>
+        <v>0.0342119069593094</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>WOO</t>
+          <t>Holo</t>
         </is>
       </c>
       <c r="B91" t="n">
         <v>90</v>
       </c>
       <c r="C91" t="n">
-        <v>0.2760413709747691</v>
+        <v>0.0036875115419074</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>Holo</t>
+          <t>Bitcoin Gold</t>
         </is>
       </c>
       <c r="B92" t="n">
         <v>91</v>
       </c>
       <c r="C92" t="n">
-        <v>0.0028964692028345</v>
+        <v>35.54908280363081</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>NXM</t>
+          <t>WOO</t>
         </is>
       </c>
       <c r="B93" t="n">
         <v>92</v>
       </c>
       <c r="C93" t="n">
-        <v>75.71350556613712</v>
+        <v>0.3353212877544386</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>TrueUSD</t>
+          <t>Telcoin</t>
         </is>
       </c>
       <c r="B94" t="n">
         <v>93</v>
       </c>
       <c r="C94" t="n">
-        <v>1.001591030172031</v>
+        <v>0.0067318032822877</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>DeXe</t>
+          <t>Enjin Coin</t>
         </is>
       </c>
       <c r="B95" t="n">
         <v>94</v>
       </c>
       <c r="C95" t="n">
-        <v>8.643956462393321</v>
+        <v>0.3460187290980695</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>Reserve Rights</t>
+          <t>Theta Fuel</t>
         </is>
       </c>
       <c r="B96" t="n">
         <v>95</v>
       </c>
       <c r="C96" t="n">
-        <v>0.009017443943484801</v>
+        <v>0.0902310787773416</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>Zilliqa</t>
+          <t>Livepeer</t>
         </is>
       </c>
       <c r="B97" t="n">
         <v>96</v>
       </c>
       <c r="C97" t="n">
-        <v>0.02491895061678</v>
+        <v>16.42672815791765</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>Golem</t>
+          <t>IoTeX</t>
         </is>
       </c>
       <c r="B98" t="n">
         <v>97</v>
       </c>
       <c r="C98" t="n">
-        <v>0.4778649501424878</v>
+        <v>0.0631239193988599</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>Trust Wallet Token</t>
+          <t>DeXe</t>
         </is>
       </c>
       <c r="B99" t="n">
         <v>98</v>
       </c>
       <c r="C99" t="n">
-        <v>1.145727847981554</v>
+        <v>10.3290787488951</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>0x Protocol</t>
+          <t>JUST</t>
         </is>
       </c>
       <c r="B100" t="n">
         <v>99</v>
       </c>
       <c r="C100" t="n">
-        <v>0.5508921118380792</v>
+        <v>0.0583069147672488</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>IoTeX</t>
+          <t>Celo</t>
         </is>
       </c>
       <c r="B101" t="n">
         <v>100</v>
       </c>
       <c r="C101" t="n">
-        <v>0.0484214435297264</v>
+        <v>1.034056470904978</v>
       </c>
     </row>
   </sheetData>
@@ -2231,13 +2231,13 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>2048.7</v>
+        <v>2041.7</v>
       </c>
       <c r="B2" t="n">
-        <v>1.6</v>
+        <v>2.5</v>
       </c>
       <c r="C2" t="n">
-        <v>13568.5</v>
+        <v>13441</v>
       </c>
     </row>
   </sheetData>

</xml_diff>